<commit_message>
Added Graphing Scripts for Location-Session graphs
</commit_message>
<xml_diff>
--- a/analyzer/Submissions/kaushalya-feedback.xlsx
+++ b/analyzer/Submissions/kaushalya-feedback.xlsx
@@ -7,32 +7,210 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Location-Rating" sheetId="1" r:id="rId1"/>
-    <sheet name="Session-Rating" sheetId="2" r:id="rId2"/>
+    <sheet name="Feedback" sheetId="1" r:id="rId1"/>
+    <sheet name="Location-Rating" sheetId="2" r:id="rId2"/>
+    <sheet name="Session-Rating" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="65">
+  <si>
+    <t>Session Location</t>
+  </si>
+  <si>
+    <t>Food Quality</t>
+  </si>
+  <si>
+    <t>Faculty Quality</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Course Relevance</t>
+  </si>
+  <si>
+    <t>Session Name</t>
+  </si>
+  <si>
+    <t>College Code</t>
+  </si>
+  <si>
+    <t>Suggestions</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Infrastructure Quality</t>
+  </si>
+  <si>
+    <t>Branch Name</t>
+  </si>
+  <si>
+    <t>Industry Learning</t>
+  </si>
+  <si>
+    <t>Mahape</t>
+  </si>
+  <si>
+    <t>Madh Island</t>
+  </si>
+  <si>
+    <t>Vidyalankar</t>
+  </si>
+  <si>
+    <t>Shriyash shelar</t>
+  </si>
+  <si>
+    <t>Abhikrant A Malavi</t>
+  </si>
+  <si>
+    <t>Hitesh Bale</t>
+  </si>
+  <si>
+    <t>Harshit Vijay Surve</t>
+  </si>
+  <si>
+    <t>Prasad Devidas Kevane</t>
+  </si>
+  <si>
+    <t>Bhushan s. Panje</t>
+  </si>
+  <si>
+    <t>VRUSHABH KRISHNADEV GHADAGE</t>
+  </si>
+  <si>
+    <t>bhagyodaya borade</t>
+  </si>
+  <si>
+    <t>TEJAS AJAY SAWANT</t>
+  </si>
+  <si>
+    <t>Amar Ajay Sawant</t>
+  </si>
+  <si>
+    <t>Prathamesh Genbhau Dhumal</t>
+  </si>
+  <si>
+    <t>Atul Mane</t>
+  </si>
+  <si>
+    <t>Electronics Hands-On Day 1</t>
+  </si>
+  <si>
+    <t>Industry Visit</t>
+  </si>
+  <si>
+    <t>Industry Exporsure</t>
+  </si>
+  <si>
+    <t>Project Day 2</t>
+  </si>
+  <si>
+    <t>Life Skills Day 2</t>
+  </si>
+  <si>
+    <t>GD and Interview</t>
+  </si>
+  <si>
+    <t>Electronics Hands-On Day 6</t>
+  </si>
+  <si>
+    <t>Computer Hands-On Day 3</t>
+  </si>
+  <si>
+    <t>Electronics Hands-On Day 2</t>
+  </si>
+  <si>
+    <t>Computer Hands-On Day 1</t>
+  </si>
+  <si>
+    <t>Computer Hands-On Day 4</t>
+  </si>
+  <si>
+    <t>Communication Skills Day 1</t>
+  </si>
+  <si>
+    <t>935</t>
+  </si>
+  <si>
+    <t>1548</t>
+  </si>
+  <si>
+    <t>1509</t>
+  </si>
+  <si>
+    <t>1146</t>
+  </si>
+  <si>
+    <t>1763</t>
+  </si>
+  <si>
+    <t>522</t>
+  </si>
+  <si>
+    <t>1736</t>
+  </si>
+  <si>
+    <t>kstud00096</t>
+  </si>
+  <si>
+    <t>kstud00076</t>
+  </si>
+  <si>
+    <t>kstud00071</t>
+  </si>
+  <si>
+    <t>kstud00001</t>
+  </si>
+  <si>
+    <t>kstud00085</t>
+  </si>
+  <si>
+    <t>kstud00087</t>
+  </si>
+  <si>
+    <t>kstud00081</t>
+  </si>
+  <si>
+    <t>kstud00008</t>
+  </si>
+  <si>
+    <t>kstud00091</t>
+  </si>
+  <si>
+    <t>kstud00005</t>
+  </si>
+  <si>
+    <t>kstud00007</t>
+  </si>
+  <si>
+    <t>kstud00067</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Computer Engineering</t>
+  </si>
+  <si>
+    <t>Electrical and Electronic Engineering</t>
+  </si>
   <si>
     <t>Faculty Rating</t>
-  </si>
-  <si>
-    <t>Food Quality</t>
-  </si>
-  <si>
-    <t>Course Relevance</t>
-  </si>
-  <si>
-    <t>Industry Exporsure</t>
-  </si>
-  <si>
-    <t>Life Skills Day 2</t>
-  </si>
-  <si>
-    <t>Project Day 2</t>
   </si>
 </sst>
 </file>
@@ -390,13 +568,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:13">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -406,47 +584,557 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>12</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>1.333333333333333</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>0</v>
+      <c r="B3" t="s">
+        <v>13</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>2.666666666666667</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>0</v>
+      <c r="B4" t="s">
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" t="s">
+        <v>59</v>
+      </c>
+      <c r="L6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" t="s">
+        <v>60</v>
+      </c>
+      <c r="L7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K8" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" t="s">
+        <v>60</v>
+      </c>
+      <c r="L10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" t="s">
+        <v>59</v>
+      </c>
+      <c r="L11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12" t="s">
+        <v>53</v>
+      </c>
+      <c r="K12" t="s">
+        <v>61</v>
+      </c>
+      <c r="L12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" t="s">
+        <v>54</v>
+      </c>
+      <c r="K13" t="s">
+        <v>59</v>
+      </c>
+      <c r="L13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J14" t="s">
+        <v>55</v>
+      </c>
+      <c r="K14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" t="s">
+        <v>56</v>
+      </c>
+      <c r="K15" t="s">
+        <v>60</v>
+      </c>
+      <c r="L15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" t="s">
+        <v>41</v>
+      </c>
+      <c r="J16" t="s">
+        <v>57</v>
+      </c>
+      <c r="K16" t="s">
+        <v>58</v>
+      </c>
+      <c r="L16" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -464,13 +1152,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -478,13 +1166,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3.333333333333333</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -492,13 +1180,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>3.666666666666667</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -506,12 +1194,186 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>3.333333333333333</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
+        <v>1.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>1.5</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>1.5</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>5</v>
+      </c>
+      <c r="M3">
+        <v>2.666666666666667</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>2.5</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
         <v>1</v>
       </c>
     </row>

</xml_diff>